<commit_message>
update new graphs_ 13_03
</commit_message>
<xml_diff>
--- a/deloitte_productivity_project/data/raw_data/sic07_identifer.xlsx
+++ b/deloitte_productivity_project/data/raw_data/sic07_identifer.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CodeClan\Project\deloitte_productivity_project\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67050937-41E7-4EE2-A946-2E415DCCF55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A36AF7-627F-4C99-BCF6-946A32A553B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15840" xr2:uid="{4E3078D2-B5AF-4302-BDEF-8312D8379BA3}"/>
+    <workbookView xWindow="28680" yWindow="-285" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4E3078D2-B5AF-4302-BDEF-8312D8379BA3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="168">
   <si>
     <t>Whole Economy</t>
   </si>
@@ -486,6 +487,57 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>sic_cat</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -846,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938CC503-024A-498A-B648-6B640453C838}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,4 +1681,195 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E533E9-AE60-439B-92A1-3DD2DE8D1360}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>